<commit_message>
creating histograms for new data
</commit_message>
<xml_diff>
--- a/clusters_at_multiple_snapshots/fire2_chemistry_analysis_multiple_snapshots/clusters_metallicities_b4n6.xlsx
+++ b/clusters_at_multiple_snapshots/fire2_chemistry_analysis_multiple_snapshots/clusters_metallicities_b4n6.xlsx
@@ -2249,7 +2249,7 @@
         <v>7</v>
       </c>
       <c r="C72">
-        <v>9.186313053334105</v>
+        <v>9.186313053334104</v>
       </c>
       <c r="D72">
         <v>-0.2360118165510901</v>
@@ -4355,7 +4355,7 @@
         <v>9</v>
       </c>
       <c r="C153">
-        <v>6.611398608039459</v>
+        <v>6.611398608039458</v>
       </c>
       <c r="D153">
         <v>-0.1934107401777784</v>

</xml_diff>